<commit_message>
ohtani back on top after running with data cleaned players csv
</commit_message>
<xml_diff>
--- a/players.xlsx
+++ b/players.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lu516e\source\repos\aflynn0213\FantasyPlayerEvaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aflyn\repos\FantasyPlayerEvaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFE6854-E5E0-4682-B445-DBD2DFAF3BCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C3C147-43DF-4077-930B-9B8169EAF832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,19 @@
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">players!$A$1:$AU$400</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2430,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O367" workbookViewId="0">
-      <selection activeCell="AL395" sqref="AL395"/>
+    <sheetView tabSelected="1" topLeftCell="X183" workbookViewId="0">
+      <selection activeCell="AU190" sqref="AU190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2697,11 +2710,11 @@
         <v>4.5</v>
       </c>
       <c r="AU2" t="str">
-        <f>IF(AND(ISBLANK(AC2),ISBLANK(AD2)),"",SUM(AC2,AD2))</f>
+        <f t="shared" ref="AU2:AU65" si="0">IF(SUM(AC2,AD2)&lt;1,"",SUM(AC2,AD2))</f>
         <v/>
       </c>
       <c r="AV2" t="str">
-        <f t="shared" ref="AV2:AV65" si="0">IF(AB2&lt;1,"",AB2)</f>
+        <f t="shared" ref="AV2:AV65" si="1">IF(AB2&lt;1,"",AB2)</f>
         <v/>
       </c>
     </row>
@@ -2773,11 +2786,11 @@
         <v>4.3</v>
       </c>
       <c r="AU3" t="str">
-        <f t="shared" ref="AU3:AU66" si="1">IF(AND(ISBLANK(AC3),ISBLANK(AD3)),"",SUM(AC3,AD3))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="AV3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2849,11 +2862,11 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="AU4" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV4" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV4" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -2925,11 +2938,11 @@
         <v>4</v>
       </c>
       <c r="AU5" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV5" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV5" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3001,11 +3014,11 @@
         <v>4</v>
       </c>
       <c r="AU6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV6" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV6" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3077,11 +3090,11 @@
         <v>3.9</v>
       </c>
       <c r="AU7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV7" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV7" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3153,11 +3166,11 @@
         <v>3.8</v>
       </c>
       <c r="AU8" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV8" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV8" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3229,11 +3242,11 @@
         <v>3.7</v>
       </c>
       <c r="AU9" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV9" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV9" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3305,11 +3318,11 @@
         <v>3.4</v>
       </c>
       <c r="AU10" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV10" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3381,11 +3394,11 @@
         <v>3.4</v>
       </c>
       <c r="AU11" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV11" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV11" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3457,11 +3470,11 @@
         <v>3.4</v>
       </c>
       <c r="AU12" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV12" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV12" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3533,11 +3546,11 @@
         <v>3.3</v>
       </c>
       <c r="AU13" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV13" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV13" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3609,11 +3622,11 @@
         <v>3.3</v>
       </c>
       <c r="AU14" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV14" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV14" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3685,11 +3698,11 @@
         <v>3.2</v>
       </c>
       <c r="AU15" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV15" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV15" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3761,11 +3774,11 @@
         <v>3.2</v>
       </c>
       <c r="AU16" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV16" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV16" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3837,11 +3850,11 @@
         <v>3.2</v>
       </c>
       <c r="AU17" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV17" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV17" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3913,11 +3926,11 @@
         <v>3.2</v>
       </c>
       <c r="AU18" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV18" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV18" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -3989,11 +4002,11 @@
         <v>3.1</v>
       </c>
       <c r="AU19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV19" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV19" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4065,11 +4078,11 @@
         <v>3.1</v>
       </c>
       <c r="AU20" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV20" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV20" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4141,11 +4154,11 @@
         <v>3.1</v>
       </c>
       <c r="AU21" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV21" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV21" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4217,11 +4230,11 @@
         <v>3.1</v>
       </c>
       <c r="AU22" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV22" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV22" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4293,11 +4306,11 @@
         <v>3</v>
       </c>
       <c r="AU23" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV23" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV23" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4369,11 +4382,11 @@
         <v>3</v>
       </c>
       <c r="AU24" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV24" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV24" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4445,11 +4458,11 @@
         <v>3</v>
       </c>
       <c r="AU25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV25" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV25" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4521,11 +4534,11 @@
         <v>3</v>
       </c>
       <c r="AU26" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV26" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV26" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4597,11 +4610,11 @@
         <v>3</v>
       </c>
       <c r="AU27" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV27" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV27" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4673,11 +4686,11 @@
         <v>3</v>
       </c>
       <c r="AU28" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV28" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV28" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4749,11 +4762,11 @@
         <v>2.8</v>
       </c>
       <c r="AU29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV29" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV29" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4825,11 +4838,11 @@
         <v>2.8</v>
       </c>
       <c r="AU30" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV30" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV30" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4901,11 +4914,11 @@
         <v>2.8</v>
       </c>
       <c r="AU31" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV31" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV31" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -4977,11 +4990,11 @@
         <v>2.8</v>
       </c>
       <c r="AU32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV32" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV32" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5053,11 +5066,11 @@
         <v>2.7</v>
       </c>
       <c r="AU33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV33" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV33" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5129,11 +5142,11 @@
         <v>2.7</v>
       </c>
       <c r="AU34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV34" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV34" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5205,11 +5218,11 @@
         <v>2.7</v>
       </c>
       <c r="AU35" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV35" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV35" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5281,11 +5294,11 @@
         <v>2.6</v>
       </c>
       <c r="AU36" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV36" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV36" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5357,11 +5370,11 @@
         <v>2.6</v>
       </c>
       <c r="AU37" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV37" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV37" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5433,11 +5446,11 @@
         <v>2.6</v>
       </c>
       <c r="AU38" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV38" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV38" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5509,11 +5522,11 @@
         <v>2.5</v>
       </c>
       <c r="AU39" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV39" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV39" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5585,11 +5598,11 @@
         <v>2.5</v>
       </c>
       <c r="AU40" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV40" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV40" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5661,11 +5674,11 @@
         <v>2.4</v>
       </c>
       <c r="AU41" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV41" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV41" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5737,11 +5750,11 @@
         <v>2.4</v>
       </c>
       <c r="AU42" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV42" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV42" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5813,11 +5826,11 @@
         <v>2.4</v>
       </c>
       <c r="AU43" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV43" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV43" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5889,11 +5902,11 @@
         <v>2.4</v>
       </c>
       <c r="AU44" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV44" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV44" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -5965,11 +5978,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU45" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV45" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV45" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6041,11 +6054,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU46" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV46" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV46" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6117,11 +6130,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU47" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV47" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV47" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6193,11 +6206,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU48" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV48" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV48" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6269,11 +6282,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU49" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV49" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV49" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6345,11 +6358,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU50" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV50" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV50" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6421,11 +6434,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU51" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV51" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV51" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6497,11 +6510,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU52" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV52" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV52" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6573,11 +6586,11 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="AU53" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV53" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV53" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6649,11 +6662,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AU54" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV54" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV54" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6725,11 +6738,11 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="AU55" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV55" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV55" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -6869,12 +6882,12 @@
       <c r="AT56">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AU56">
+      <c r="AU56" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV56">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="AV56">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -6946,11 +6959,11 @@
         <v>2.1</v>
       </c>
       <c r="AU57" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV57" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV57" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7022,11 +7035,11 @@
         <v>2.1</v>
       </c>
       <c r="AU58" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV58" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV58" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7098,11 +7111,11 @@
         <v>2.1</v>
       </c>
       <c r="AU59" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV59" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV59" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7174,11 +7187,11 @@
         <v>2.1</v>
       </c>
       <c r="AU60" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV60" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV60" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7250,11 +7263,11 @@
         <v>2.1</v>
       </c>
       <c r="AU61" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV61" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV61" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7326,11 +7339,11 @@
         <v>2</v>
       </c>
       <c r="AU62" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV62" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV62" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7402,11 +7415,11 @@
         <v>2</v>
       </c>
       <c r="AU63" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV63" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV63" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7478,11 +7491,11 @@
         <v>2</v>
       </c>
       <c r="AU64" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV64" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV64" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7554,11 +7567,11 @@
         <v>2</v>
       </c>
       <c r="AU65" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AV65" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="AV65" t="str">
-        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -7630,11 +7643,11 @@
         <v>2</v>
       </c>
       <c r="AU66" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="AU66:AU129" si="2">IF(SUM(AC66,AD66)&lt;1,"",SUM(AC66,AD66))</f>
         <v/>
       </c>
       <c r="AV66" t="str">
-        <f t="shared" ref="AV66:AV129" si="2">IF(AB66&lt;1,"",AB66)</f>
+        <f t="shared" ref="AV66:AV129" si="3">IF(AB66&lt;1,"",AB66)</f>
         <v/>
       </c>
     </row>
@@ -7706,11 +7719,11 @@
         <v>1.9</v>
       </c>
       <c r="AU67" t="str">
-        <f t="shared" ref="AU67:AU130" si="3">IF(AND(ISBLANK(AC67),ISBLANK(AD67)),"",SUM(AC67,AD67))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="AV67" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
@@ -7782,11 +7795,11 @@
         <v>1.9</v>
       </c>
       <c r="AU68" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV68" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV68" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -7858,11 +7871,11 @@
         <v>1.9</v>
       </c>
       <c r="AU69" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV69" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV69" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -7934,11 +7947,11 @@
         <v>1.9</v>
       </c>
       <c r="AU70" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV70" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV70" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8010,11 +8023,11 @@
         <v>1.9</v>
       </c>
       <c r="AU71" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV71" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV71" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8086,11 +8099,11 @@
         <v>1.9</v>
       </c>
       <c r="AU72" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV72" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV72" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8162,11 +8175,11 @@
         <v>1.9</v>
       </c>
       <c r="AU73" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV73" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV73" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8238,11 +8251,11 @@
         <v>1.9</v>
       </c>
       <c r="AU74" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV74" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV74" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8314,11 +8327,11 @@
         <v>1.9</v>
       </c>
       <c r="AU75" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV75" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV75" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8390,11 +8403,11 @@
         <v>1.9</v>
       </c>
       <c r="AU76" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV76" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV76" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8466,11 +8479,11 @@
         <v>1.9</v>
       </c>
       <c r="AU77" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV77" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV77" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8542,11 +8555,11 @@
         <v>1.8</v>
       </c>
       <c r="AU78" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV78" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV78" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8618,11 +8631,11 @@
         <v>1.8</v>
       </c>
       <c r="AU79" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV79" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV79" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8694,11 +8707,11 @@
         <v>1.8</v>
       </c>
       <c r="AU80" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV80" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV80" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8770,11 +8783,11 @@
         <v>1.8</v>
       </c>
       <c r="AU81" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV81" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV81" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8846,11 +8859,11 @@
         <v>1.8</v>
       </c>
       <c r="AU82" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV82" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV82" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8922,11 +8935,11 @@
         <v>1.8</v>
       </c>
       <c r="AU83" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV83" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV83" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -8998,11 +9011,11 @@
         <v>1.8</v>
       </c>
       <c r="AU84" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV84" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV84" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9074,11 +9087,11 @@
         <v>1.8</v>
       </c>
       <c r="AU85" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV85" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV85" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9150,11 +9163,11 @@
         <v>1.8</v>
       </c>
       <c r="AU86" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV86" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV86" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9226,11 +9239,11 @@
         <v>1.7</v>
       </c>
       <c r="AU87" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV87" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV87" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9302,11 +9315,11 @@
         <v>1.7</v>
       </c>
       <c r="AU88" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV88" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV88" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9378,11 +9391,11 @@
         <v>1.7</v>
       </c>
       <c r="AU89" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV89" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV89" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9454,11 +9467,11 @@
         <v>1.7</v>
       </c>
       <c r="AU90" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV90" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV90" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9530,11 +9543,11 @@
         <v>1.7</v>
       </c>
       <c r="AU91" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV91" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV91" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9606,11 +9619,11 @@
         <v>1.7</v>
       </c>
       <c r="AU92" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV92" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV92" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9682,11 +9695,11 @@
         <v>1.6</v>
       </c>
       <c r="AU93" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV93" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV93" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9758,11 +9771,11 @@
         <v>1.6</v>
       </c>
       <c r="AU94" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV94" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV94" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9834,11 +9847,11 @@
         <v>1.6</v>
       </c>
       <c r="AU95" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV95" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV95" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9910,11 +9923,11 @@
         <v>1.6</v>
       </c>
       <c r="AU96" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV96" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV96" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -9986,11 +9999,11 @@
         <v>1.6</v>
       </c>
       <c r="AU97" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV97" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV97" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10062,11 +10075,11 @@
         <v>1.6</v>
       </c>
       <c r="AU98" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV98" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV98" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10138,11 +10151,11 @@
         <v>1.6</v>
       </c>
       <c r="AU99" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV99" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV99" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10214,11 +10227,11 @@
         <v>1.6</v>
       </c>
       <c r="AU100" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV100" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV100" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10290,11 +10303,11 @@
         <v>1.6</v>
       </c>
       <c r="AU101" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV101" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV101" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10366,11 +10379,11 @@
         <v>1.6</v>
       </c>
       <c r="AU102" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV102" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV102" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10442,11 +10455,11 @@
         <v>1.6</v>
       </c>
       <c r="AU103" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV103" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV103" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10518,11 +10531,11 @@
         <v>1.6</v>
       </c>
       <c r="AU104" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV104" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV104" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10594,11 +10607,11 @@
         <v>1.6</v>
       </c>
       <c r="AU105" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV105" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV105" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10670,11 +10683,11 @@
         <v>1.5</v>
       </c>
       <c r="AU106" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV106" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV106" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10746,11 +10759,11 @@
         <v>1.5</v>
       </c>
       <c r="AU107" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV107" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV107" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10822,11 +10835,11 @@
         <v>1.5</v>
       </c>
       <c r="AU108" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV108" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV108" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10898,11 +10911,11 @@
         <v>1.5</v>
       </c>
       <c r="AU109" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV109" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV109" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -10974,11 +10987,11 @@
         <v>1.5</v>
       </c>
       <c r="AU110" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV110" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV110" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11050,11 +11063,11 @@
         <v>1.5</v>
       </c>
       <c r="AU111" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV111" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV111" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11126,11 +11139,11 @@
         <v>1.5</v>
       </c>
       <c r="AU112" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV112" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV112" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11202,11 +11215,11 @@
         <v>1.5</v>
       </c>
       <c r="AU113" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV113" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV113" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11278,11 +11291,11 @@
         <v>1.5</v>
       </c>
       <c r="AU114" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV114" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV114" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11354,11 +11367,11 @@
         <v>1.4</v>
       </c>
       <c r="AU115" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV115" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV115" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11430,11 +11443,11 @@
         <v>1.4</v>
       </c>
       <c r="AU116" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV116" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV116" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11506,11 +11519,11 @@
         <v>1.4</v>
       </c>
       <c r="AU117" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV117" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV117" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11582,11 +11595,11 @@
         <v>1.4</v>
       </c>
       <c r="AU118" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV118" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV118" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11658,11 +11671,11 @@
         <v>1.4</v>
       </c>
       <c r="AU119" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV119" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV119" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11734,11 +11747,11 @@
         <v>1.4</v>
       </c>
       <c r="AU120" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV120" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV120" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11810,11 +11823,11 @@
         <v>1.4</v>
       </c>
       <c r="AU121" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV121" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV121" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11886,11 +11899,11 @@
         <v>1.4</v>
       </c>
       <c r="AU122" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV122" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV122" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -11962,11 +11975,11 @@
         <v>1.4</v>
       </c>
       <c r="AU123" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV123" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV123" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12038,11 +12051,11 @@
         <v>1.4</v>
       </c>
       <c r="AU124" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV124" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV124" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12114,11 +12127,11 @@
         <v>1.4</v>
       </c>
       <c r="AU125" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV125" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV125" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12190,11 +12203,11 @@
         <v>1.4</v>
       </c>
       <c r="AU126" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV126" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV126" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12266,11 +12279,11 @@
         <v>1.4</v>
       </c>
       <c r="AU127" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV127" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV127" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12342,11 +12355,11 @@
         <v>1.4</v>
       </c>
       <c r="AU128" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV128" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV128" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12418,11 +12431,11 @@
         <v>1.3</v>
       </c>
       <c r="AU129" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AV129" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="AV129" t="str">
-        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -12494,11 +12507,11 @@
         <v>1.3</v>
       </c>
       <c r="AU130" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AU130:AU193" si="4">IF(SUM(AC130,AD130)&lt;1,"",SUM(AC130,AD130))</f>
         <v/>
       </c>
       <c r="AV130" t="str">
-        <f t="shared" ref="AV130:AV193" si="4">IF(AB130&lt;1,"",AB130)</f>
+        <f t="shared" ref="AV130:AV193" si="5">IF(AB130&lt;1,"",AB130)</f>
         <v/>
       </c>
     </row>
@@ -12570,11 +12583,11 @@
         <v>1.3</v>
       </c>
       <c r="AU131" t="str">
-        <f t="shared" ref="AU131:AU194" si="5">IF(AND(ISBLANK(AC131),ISBLANK(AD131)),"",SUM(AC131,AD131))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AV131" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
@@ -12646,11 +12659,11 @@
         <v>1.3</v>
       </c>
       <c r="AU132" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV132" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV132" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -12722,11 +12735,11 @@
         <v>1.3</v>
       </c>
       <c r="AU133" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV133" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV133" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -12798,11 +12811,11 @@
         <v>1.3</v>
       </c>
       <c r="AU134" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV134" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV134" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -12874,11 +12887,11 @@
         <v>1.3</v>
       </c>
       <c r="AU135" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV135" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV135" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -12950,11 +12963,11 @@
         <v>1.3</v>
       </c>
       <c r="AU136" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV136" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV136" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13026,11 +13039,11 @@
         <v>1.3</v>
       </c>
       <c r="AU137" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV137" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV137" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13102,11 +13115,11 @@
         <v>1.3</v>
       </c>
       <c r="AU138" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV138" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV138" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13178,11 +13191,11 @@
         <v>1.3</v>
       </c>
       <c r="AU139" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV139" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV139" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13254,11 +13267,11 @@
         <v>1.3</v>
       </c>
       <c r="AU140" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV140" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV140" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13330,11 +13343,11 @@
         <v>1.2</v>
       </c>
       <c r="AU141" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV141" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV141" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13406,11 +13419,11 @@
         <v>1.2</v>
       </c>
       <c r="AU142" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV142" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV142" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13482,11 +13495,11 @@
         <v>1.2</v>
       </c>
       <c r="AU143" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV143" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV143" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13558,11 +13571,11 @@
         <v>1.2</v>
       </c>
       <c r="AU144" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV144" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV144" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13634,11 +13647,11 @@
         <v>1.2</v>
       </c>
       <c r="AU145" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV145" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV145" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13710,11 +13723,11 @@
         <v>1.2</v>
       </c>
       <c r="AU146" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV146" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV146" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13786,11 +13799,11 @@
         <v>1.2</v>
       </c>
       <c r="AU147" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV147" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV147" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13862,11 +13875,11 @@
         <v>1.2</v>
       </c>
       <c r="AU148" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV148" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV148" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -13938,11 +13951,11 @@
         <v>1.2</v>
       </c>
       <c r="AU149" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV149" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV149" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14014,11 +14027,11 @@
         <v>1.2</v>
       </c>
       <c r="AU150" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV150" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV150" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14090,11 +14103,11 @@
         <v>1.2</v>
       </c>
       <c r="AU151" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV151" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV151" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14166,11 +14179,11 @@
         <v>1.2</v>
       </c>
       <c r="AU152" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV152" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV152" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14242,11 +14255,11 @@
         <v>1.2</v>
       </c>
       <c r="AU153" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV153" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV153" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14318,11 +14331,11 @@
         <v>1.2</v>
       </c>
       <c r="AU154" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV154" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV154" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14394,11 +14407,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU155" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV155" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV155" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14470,11 +14483,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU156" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV156" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV156" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14546,11 +14559,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU157" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV157" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV157" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14622,11 +14635,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU158" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV158" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV158" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14698,11 +14711,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU159" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV159" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV159" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14774,11 +14787,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU160" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV160" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV160" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14850,11 +14863,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU161" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV161" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV161" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -14926,11 +14939,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU162" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV162" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV162" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15002,11 +15015,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU163" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV163" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV163" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15078,11 +15091,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU164" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV164" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV164" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15154,11 +15167,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU165" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV165" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV165" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15230,11 +15243,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU166" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV166" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV166" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15306,11 +15319,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU167" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV167" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV167" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15382,11 +15395,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU168" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV168" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV168" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15458,11 +15471,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU169" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV169" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV169" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15534,11 +15547,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU170" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV170" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV170" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15610,11 +15623,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="AU171" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV171" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV171" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15686,11 +15699,11 @@
         <v>1</v>
       </c>
       <c r="AU172" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV172" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV172" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15762,11 +15775,11 @@
         <v>1</v>
       </c>
       <c r="AU173" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV173" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV173" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15838,11 +15851,11 @@
         <v>1</v>
       </c>
       <c r="AU174" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV174" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV174" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15914,11 +15927,11 @@
         <v>1</v>
       </c>
       <c r="AU175" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV175" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV175" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -15990,11 +16003,11 @@
         <v>1</v>
       </c>
       <c r="AU176" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV176" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV176" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16066,11 +16079,11 @@
         <v>1</v>
       </c>
       <c r="AU177" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV177" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV177" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16142,11 +16155,11 @@
         <v>1</v>
       </c>
       <c r="AU178" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV178" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV178" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16218,11 +16231,11 @@
         <v>1</v>
       </c>
       <c r="AU179" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV179" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV179" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16294,11 +16307,11 @@
         <v>1</v>
       </c>
       <c r="AU180" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV180" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV180" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16370,11 +16383,11 @@
         <v>1</v>
       </c>
       <c r="AU181" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV181" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV181" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16446,11 +16459,11 @@
         <v>1</v>
       </c>
       <c r="AU182" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV182" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV182" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16522,11 +16535,11 @@
         <v>1</v>
       </c>
       <c r="AU183" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV183" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV183" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16598,11 +16611,11 @@
         <v>1</v>
       </c>
       <c r="AU184" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV184" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV184" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16674,11 +16687,11 @@
         <v>1</v>
       </c>
       <c r="AU185" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV185" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV185" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16750,11 +16763,11 @@
         <v>1</v>
       </c>
       <c r="AU186" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV186" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV186" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16826,11 +16839,11 @@
         <v>1</v>
       </c>
       <c r="AU187" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV187" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV187" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16902,11 +16915,11 @@
         <v>1</v>
       </c>
       <c r="AU188" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV188" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV188" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -16978,11 +16991,11 @@
         <v>0.9</v>
       </c>
       <c r="AU189" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV189" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV189" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -17054,11 +17067,11 @@
         <v>0.9</v>
       </c>
       <c r="AU190" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV190" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV190" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -17130,11 +17143,11 @@
         <v>0.9</v>
       </c>
       <c r="AU191" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV191" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV191" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -17206,11 +17219,11 @@
         <v>0.9</v>
       </c>
       <c r="AU192" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV192" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV192" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -17282,11 +17295,11 @@
         <v>0.9</v>
       </c>
       <c r="AU193" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="AV193" t="str">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AV193" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -17358,11 +17371,11 @@
         <v>0.9</v>
       </c>
       <c r="AU194" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="AU194:AU201" si="6">IF(SUM(AC194,AD194)&lt;1,"",SUM(AC194,AD194))</f>
         <v/>
       </c>
       <c r="AV194" t="str">
-        <f t="shared" ref="AV194:AV257" si="6">IF(AB194&lt;1,"",AB194)</f>
+        <f t="shared" ref="AV194:AV257" si="7">IF(AB194&lt;1,"",AB194)</f>
         <v/>
       </c>
     </row>
@@ -17434,11 +17447,11 @@
         <v>0.9</v>
       </c>
       <c r="AU195" t="str">
-        <f t="shared" ref="AU195:AU258" si="7">IF(AND(ISBLANK(AC195),ISBLANK(AD195)),"",SUM(AC195,AD195))</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AV195" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -17510,11 +17523,11 @@
         <v>0.9</v>
       </c>
       <c r="AU196" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV196" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV196" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17586,11 +17599,11 @@
         <v>0.9</v>
       </c>
       <c r="AU197" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV197" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV197" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17662,11 +17675,11 @@
         <v>0.9</v>
       </c>
       <c r="AU198" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV198" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV198" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17738,11 +17751,11 @@
         <v>0.9</v>
       </c>
       <c r="AU199" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV199" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV199" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17814,11 +17827,11 @@
         <v>0.9</v>
       </c>
       <c r="AU200" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV200" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV200" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17890,11 +17903,11 @@
         <v>0.9</v>
       </c>
       <c r="AU201" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="AV201" t="str">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AV201" t="str">
-        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -17982,7 +17995,7 @@
         <v/>
       </c>
       <c r="AV202">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16</v>
       </c>
     </row>
@@ -18070,7 +18083,7 @@
         <v/>
       </c>
       <c r="AV203">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -18158,7 +18171,7 @@
         <v/>
       </c>
       <c r="AV204">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -18246,7 +18259,7 @@
         <v/>
       </c>
       <c r="AV205">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -18334,7 +18347,7 @@
         <v/>
       </c>
       <c r="AV206">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -18422,7 +18435,7 @@
         <v/>
       </c>
       <c r="AV207">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -18510,7 +18523,7 @@
         <v/>
       </c>
       <c r="AV208">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -18598,7 +18611,7 @@
         <v/>
       </c>
       <c r="AV209">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -18686,7 +18699,7 @@
         <v/>
       </c>
       <c r="AV210">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -18774,7 +18787,7 @@
         <v/>
       </c>
       <c r="AV211">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -18862,7 +18875,7 @@
         <v/>
       </c>
       <c r="AV212">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15</v>
       </c>
     </row>
@@ -18950,7 +18963,7 @@
         <v/>
       </c>
       <c r="AV213">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -19038,7 +19051,7 @@
         <v/>
       </c>
       <c r="AV214">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -19126,7 +19139,7 @@
         <v/>
       </c>
       <c r="AV215">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
     </row>
@@ -19214,7 +19227,7 @@
         <v/>
       </c>
       <c r="AV216">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -19302,7 +19315,7 @@
         <v/>
       </c>
       <c r="AV217">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -19390,7 +19403,7 @@
         <v/>
       </c>
       <c r="AV218">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -19478,7 +19491,7 @@
         <v/>
       </c>
       <c r="AV219">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -19566,7 +19579,7 @@
         <v/>
       </c>
       <c r="AV220">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -19654,7 +19667,7 @@
         <v/>
       </c>
       <c r="AV221">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -19742,7 +19755,7 @@
         <v/>
       </c>
       <c r="AV222">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -19830,7 +19843,7 @@
         <v/>
       </c>
       <c r="AV223">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -19918,7 +19931,7 @@
         <v/>
       </c>
       <c r="AV224">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -20006,7 +20019,7 @@
         <v/>
       </c>
       <c r="AV225">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20094,7 +20107,7 @@
         <v/>
       </c>
       <c r="AV226">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20182,7 +20195,7 @@
         <v/>
       </c>
       <c r="AV227">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -20270,7 +20283,7 @@
         <v/>
       </c>
       <c r="AV228">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -20358,7 +20371,7 @@
         <v/>
       </c>
       <c r="AV229">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20446,7 +20459,7 @@
         <v/>
       </c>
       <c r="AV230">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20534,7 +20547,7 @@
         <v/>
       </c>
       <c r="AV231">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20622,7 +20635,7 @@
         <v/>
       </c>
       <c r="AV232">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -20710,7 +20723,7 @@
         <v/>
       </c>
       <c r="AV233">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -20798,7 +20811,7 @@
         <v/>
       </c>
       <c r="AV234">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20886,7 +20899,7 @@
         <v/>
       </c>
       <c r="AV235">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -20974,7 +20987,7 @@
         <v/>
       </c>
       <c r="AV236">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21062,7 +21075,7 @@
         <v/>
       </c>
       <c r="AV237">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21150,7 +21163,7 @@
         <v/>
       </c>
       <c r="AV238">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21238,7 +21251,7 @@
         <v/>
       </c>
       <c r="AV239">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
     </row>
@@ -21326,7 +21339,7 @@
         <v/>
       </c>
       <c r="AV240">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21414,7 +21427,7 @@
         <v/>
       </c>
       <c r="AV241">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -21502,7 +21515,7 @@
         <v/>
       </c>
       <c r="AV242">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
@@ -21590,7 +21603,7 @@
         <v/>
       </c>
       <c r="AV243">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21678,7 +21691,7 @@
         <v/>
       </c>
       <c r="AV244">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -21766,7 +21779,7 @@
         <v/>
       </c>
       <c r="AV245">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
@@ -21854,7 +21867,7 @@
         <v/>
       </c>
       <c r="AV246">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -21942,7 +21955,7 @@
         <v/>
       </c>
       <c r="AV247">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7</v>
       </c>
     </row>
@@ -22030,7 +22043,7 @@
         <v/>
       </c>
       <c r="AV248">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -22118,7 +22131,7 @@
         <v/>
       </c>
       <c r="AV249">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -22206,7 +22219,7 @@
         <v/>
       </c>
       <c r="AV250">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -22294,7 +22307,7 @@
         <v/>
       </c>
       <c r="AV251">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
@@ -22382,7 +22395,7 @@
         <v/>
       </c>
       <c r="AV252">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
     </row>
@@ -22470,7 +22483,7 @@
         <v/>
       </c>
       <c r="AV253">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
@@ -22558,7 +22571,7 @@
         <v/>
       </c>
       <c r="AV254">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
@@ -22646,7 +22659,7 @@
         <v/>
       </c>
       <c r="AV255">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>8</v>
       </c>
     </row>
@@ -22734,7 +22747,7 @@
         <v/>
       </c>
       <c r="AV256">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>
@@ -22822,7 +22835,7 @@
         <v/>
       </c>
       <c r="AV257">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9</v>
       </c>
     </row>

</xml_diff>